<commit_message>
Add conflict reasoning for.
</commit_message>
<xml_diff>
--- a/LOI/COI/COI-abbasi.xlsx
+++ b/LOI/COI/COI-abbasi.xlsx
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="104">
-  <si>
-    <t xml:space="preserve"> U. Tenn. Knoxville</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="92">
   <si>
     <t xml:space="preserve"> UNM</t>
   </si>
@@ -81,9 +78,6 @@
     <t>R.</t>
   </si>
   <si>
-    <t>K. L.</t>
-  </si>
-  <si>
     <t>Z.</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>Wolf</t>
   </si>
   <si>
-    <t>Choudhary</t>
-  </si>
-  <si>
     <t>Chang</t>
   </si>
   <si>
@@ -120,12 +111,6 @@
     <t>Oldfield</t>
   </si>
   <si>
-    <t>Beck</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
     <t>Lin</t>
   </si>
   <si>
@@ -147,9 +132,6 @@
     <t>McCormick</t>
   </si>
   <si>
-    <t>NWU</t>
-  </si>
-  <si>
     <t>Bremer</t>
   </si>
   <si>
@@ -210,9 +192,6 @@
     <t>Shalf</t>
   </si>
   <si>
-    <t>Shoshani</t>
-  </si>
-  <si>
     <t>Wu</t>
   </si>
   <si>
@@ -246,30 +225,15 @@
     <t>SNL</t>
   </si>
   <si>
-    <t>Brown</t>
-  </si>
-  <si>
     <t>Kolla</t>
   </si>
   <si>
     <t>Emory</t>
   </si>
   <si>
-    <t>U.C. Davis</t>
-  </si>
-  <si>
-    <t>Ross</t>
-  </si>
-  <si>
     <t>Georgia Tech</t>
   </si>
   <si>
-    <t>Worley</t>
-  </si>
-  <si>
-    <t>Prahbat</t>
-  </si>
-  <si>
     <t>Ohio State</t>
   </si>
   <si>
@@ -282,21 +246,12 @@
     <t>Widener</t>
   </si>
   <si>
-    <t>Yuan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T. </t>
-  </si>
-  <si>
     <t>Pirkelbauer</t>
   </si>
   <si>
     <t>UAB</t>
   </si>
   <si>
-    <t>Ainsworth</t>
-  </si>
-  <si>
     <t xml:space="preserve">M. </t>
   </si>
   <si>
@@ -334,6 +289,15 @@
   </si>
   <si>
     <t>Carey</t>
+  </si>
+  <si>
+    <t>co-author</t>
+  </si>
+  <si>
+    <t>collaborator</t>
+  </si>
+  <si>
+    <t>advisor</t>
   </si>
 </sst>
 </file>
@@ -728,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J235"/>
+  <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -743,556 +707,614 @@
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1">
+    <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="D14" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75">
+      <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D17" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75">
-      <c r="A20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>48</v>
+      <c r="D21" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>82</v>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>53</v>
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>56</v>
+      <c r="A25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6" t="s">
-        <v>52</v>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>44</v>
+      <c r="D28" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>53</v>
+      <c r="A29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>76</v>
+      <c r="A30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>60</v>
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="A32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B46" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>90</v>
+      </c>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="1"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="1"/>
+      <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75">
-      <c r="A50" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I50" s="3"/>
+      <c r="A49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="1"/>
+      <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1"/>
@@ -1302,41 +1324,49 @@
       <c r="A52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" ht="15.75">
       <c r="A53" s="1"/>
       <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75">
       <c r="A54" s="1"/>
       <c r="C54" s="1"/>
+      <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" ht="15.75">
       <c r="A56" s="1"/>
       <c r="C56" s="1"/>
+      <c r="H56" s="3"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" ht="15.75">
       <c r="A58" s="1"/>
       <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75">
       <c r="A59" s="1"/>
       <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75">
       <c r="A60" s="1"/>
       <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75">
       <c r="A61" s="1"/>
       <c r="C61" s="1"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
     </row>
     <row r="62" spans="1:9" ht="15.75">
       <c r="A62" s="1"/>
@@ -1344,47 +1374,59 @@
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:9" ht="15.75">
-      <c r="A63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="1"/>
-      <c r="C64" s="1"/>
+    <row r="64" spans="1:9" ht="15.75">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
     </row>
     <row r="65" spans="1:9" ht="15.75">
-      <c r="A65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="1"/>
-      <c r="C66" s="1"/>
+    <row r="66" spans="1:9" ht="15.75">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="H66" s="3"/>
     </row>
     <row r="67" spans="1:9" ht="15.75">
-      <c r="A67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
       <c r="H67" s="3"/>
     </row>
     <row r="68" spans="1:9" ht="15.75">
-      <c r="A68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
       <c r="H68" s="3"/>
     </row>
     <row r="69" spans="1:9" ht="15.75">
-      <c r="A69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
       <c r="H69" s="3"/>
     </row>
     <row r="70" spans="1:9" ht="15.75">
-      <c r="A70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
     </row>
     <row r="71" spans="1:9" ht="15.75">
-      <c r="A71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:9" ht="15.75">
@@ -1392,13 +1434,13 @@
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
     </row>
     <row r="73" spans="1:9" ht="15.75">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
     </row>
     <row r="74" spans="1:9" ht="15.75">
       <c r="A74" s="3"/>
@@ -1448,25 +1490,26 @@
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
     </row>
     <row r="82" spans="1:9" ht="15.75">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
-      <c r="H82" s="3"/>
+      <c r="H82" s="4"/>
     </row>
     <row r="83" spans="1:9" ht="15.75">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
     </row>
     <row r="84" spans="1:9" ht="15.75">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
     </row>
     <row r="85" spans="1:9" ht="15.75">
       <c r="A85" s="3"/>
@@ -1479,6 +1522,7 @@
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
     </row>
     <row r="87" spans="1:9" ht="15.75">
       <c r="A87" s="3"/>
@@ -1491,7 +1535,6 @@
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
     </row>
     <row r="89" spans="1:9" ht="15.75">
       <c r="A89" s="3"/>
@@ -1509,21 +1552,19 @@
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
-      <c r="H91" s="4"/>
+      <c r="H91" s="3"/>
     </row>
     <row r="92" spans="1:9" ht="15.75">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="H92" s="3"/>
-      <c r="I92" s="3"/>
     </row>
     <row r="93" spans="1:9" ht="15.75">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="H93" s="3"/>
-      <c r="I93" s="3"/>
     </row>
     <row r="94" spans="1:9" ht="15.75">
       <c r="A94" s="3"/>
@@ -1536,7 +1577,6 @@
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
     </row>
     <row r="96" spans="1:9" ht="15.75">
       <c r="A96" s="3"/>
@@ -1573,237 +1613,228 @@
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
     </row>
     <row r="102" spans="1:9" ht="15.75">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
     </row>
     <row r="103" spans="1:9" ht="15.75">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
     </row>
     <row r="104" spans="1:9" ht="15.75">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
     </row>
     <row r="105" spans="1:9" ht="15.75">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
     </row>
     <row r="106" spans="1:9" ht="15.75">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
-      <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:9" ht="15.75">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
-      <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:9" ht="15.75">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
-      <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:9" ht="15.75">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
-      <c r="H109" s="3"/>
     </row>
     <row r="110" spans="1:9" ht="15.75">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
-      <c r="H110" s="3"/>
-      <c r="I110" s="3"/>
     </row>
     <row r="111" spans="1:9" ht="15.75">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
-      <c r="H111" s="3"/>
-      <c r="I111" s="3"/>
     </row>
     <row r="112" spans="1:9" ht="15.75">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
-      <c r="H112" s="3"/>
-      <c r="I112" s="3"/>
-    </row>
-    <row r="113" spans="1:9" ht="15.75">
+    </row>
+    <row r="113" spans="1:8" ht="15.75">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
-      <c r="H113" s="3"/>
-      <c r="I113" s="3"/>
-    </row>
-    <row r="114" spans="1:9" ht="15.75">
+    </row>
+    <row r="114" spans="1:8" ht="15.75">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
-      <c r="H114" s="3"/>
-      <c r="I114" s="3"/>
-    </row>
-    <row r="115" spans="1:9" ht="15.75">
+    </row>
+    <row r="115" spans="1:8" ht="15.75">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
     </row>
-    <row r="116" spans="1:9" ht="15.75">
+    <row r="116" spans="1:8" ht="15.75">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" spans="1:9" ht="15.75">
+    <row r="117" spans="1:8" ht="15.75">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="1:9" ht="15.75">
+    <row r="118" spans="1:8" ht="15.75">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" spans="1:9" ht="15.75">
+    <row r="119" spans="1:8" ht="15.75">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" spans="1:9" ht="15.75">
+    <row r="120" spans="1:8" ht="15.75">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" spans="1:9" ht="15.75">
+    <row r="121" spans="1:8" ht="15.75">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
-    </row>
-    <row r="122" spans="1:9" ht="15.75">
+      <c r="H121" s="5"/>
+    </row>
+    <row r="122" spans="1:8" ht="15.75">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
     </row>
-    <row r="123" spans="1:9" ht="15.75">
+    <row r="123" spans="1:8" ht="15.75">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" spans="1:9" ht="15.75">
+    <row r="124" spans="1:8" ht="15.75">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" spans="1:9" ht="15.75">
+    <row r="125" spans="1:8" ht="15.75">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" spans="1:9" ht="15.75">
+    <row r="126" spans="1:8" ht="15.75">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" spans="1:9" ht="15.75">
+    <row r="127" spans="1:8" ht="15.75">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" spans="1:9" ht="15.75">
+    <row r="128" spans="1:8" ht="15.75">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" spans="1:8" ht="15.75">
+    <row r="129" spans="1:3" ht="15.75">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" spans="1:8" ht="15.75">
+    <row r="130" spans="1:3" ht="15.75">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
-      <c r="H130" s="5"/>
-    </row>
-    <row r="131" spans="1:8" ht="15.75">
+    </row>
+    <row r="131" spans="1:3" ht="15.75">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" spans="1:8" ht="15.75">
+    <row r="132" spans="1:3" ht="15.75">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" spans="1:8" ht="15.75">
+    <row r="133" spans="1:3" ht="15.75">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
     </row>
-    <row r="134" spans="1:8" ht="15.75">
+    <row r="134" spans="1:3" ht="15.75">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" spans="1:8" ht="15.75">
+    <row r="135" spans="1:3" ht="15.75">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" spans="1:8" ht="15.75">
+    <row r="136" spans="1:3" ht="15.75">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" spans="1:8" ht="15.75">
+    <row r="137" spans="1:3" ht="15.75">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" spans="1:8" ht="15.75">
+    <row r="138" spans="1:3" ht="15.75">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" spans="1:8" ht="15.75">
+    <row r="139" spans="1:3" ht="15.75">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" spans="1:8" ht="15.75">
+    <row r="140" spans="1:3" ht="15.75">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" spans="1:8" ht="15.75">
-      <c r="A141" s="3"/>
-      <c r="B141" s="3"/>
-      <c r="C141" s="3"/>
-    </row>
-    <row r="142" spans="1:8" ht="15.75">
+    <row r="141" spans="1:3">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4"/>
+      <c r="C141" s="4"/>
+    </row>
+    <row r="142" spans="1:3" ht="15.75">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" spans="1:8" ht="15.75">
+    <row r="143" spans="1:3" ht="15.75">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
     </row>
-    <row r="144" spans="1:8" ht="15.75">
+    <row r="144" spans="1:3" ht="15.75">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -1833,10 +1864,10 @@
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
     </row>
-    <row r="150" spans="1:3">
-      <c r="A150" s="4"/>
-      <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
+    <row r="150" spans="1:3" ht="15.75">
+      <c r="A150" s="3"/>
+      <c r="B150" s="3"/>
+      <c r="C150" s="3"/>
     </row>
     <row r="151" spans="1:3" ht="15.75">
       <c r="A151" s="3"/>
@@ -1908,56 +1939,56 @@
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
     </row>
-    <row r="165" spans="1:8" ht="15.75">
-      <c r="A165" s="3"/>
-      <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
-    </row>
-    <row r="166" spans="1:8" ht="15.75">
-      <c r="A166" s="3"/>
-      <c r="B166" s="3"/>
-      <c r="C166" s="3"/>
-    </row>
-    <row r="167" spans="1:8" ht="15.75">
-      <c r="A167" s="3"/>
-      <c r="B167" s="3"/>
-      <c r="C167" s="3"/>
-    </row>
-    <row r="168" spans="1:8" ht="15.75">
-      <c r="A168" s="3"/>
-      <c r="B168" s="3"/>
-      <c r="C168" s="3"/>
-    </row>
-    <row r="169" spans="1:8" ht="15.75">
-      <c r="A169" s="3"/>
-      <c r="B169" s="3"/>
-      <c r="C169" s="3"/>
-    </row>
-    <row r="170" spans="1:8" ht="15.75">
-      <c r="A170" s="3"/>
-      <c r="B170" s="3"/>
-      <c r="C170" s="3"/>
-    </row>
-    <row r="171" spans="1:8" ht="15.75">
-      <c r="A171" s="3"/>
-      <c r="B171" s="3"/>
-      <c r="C171" s="3"/>
-    </row>
-    <row r="172" spans="1:8" ht="15.75">
-      <c r="A172" s="3"/>
-      <c r="B172" s="3"/>
-      <c r="C172" s="3"/>
-    </row>
-    <row r="173" spans="1:8" ht="15.75">
-      <c r="A173" s="3"/>
-      <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
+    <row r="165" spans="1:8">
+      <c r="A165" s="5"/>
+      <c r="B165" s="5"/>
+      <c r="C165" s="5"/>
+      <c r="H165" s="5"/>
+    </row>
+    <row r="166" spans="1:8">
+      <c r="A166" s="5"/>
+      <c r="B166" s="5"/>
+      <c r="C166" s="5"/>
+    </row>
+    <row r="167" spans="1:8">
+      <c r="A167" s="5"/>
+      <c r="B167" s="5"/>
+      <c r="C167" s="5"/>
+    </row>
+    <row r="168" spans="1:8">
+      <c r="A168" s="5"/>
+      <c r="B168" s="5"/>
+      <c r="C168" s="5"/>
+    </row>
+    <row r="169" spans="1:8">
+      <c r="A169" s="5"/>
+      <c r="B169" s="5"/>
+      <c r="C169" s="5"/>
+    </row>
+    <row r="170" spans="1:8">
+      <c r="A170" s="5"/>
+      <c r="B170" s="5"/>
+      <c r="C170" s="5"/>
+    </row>
+    <row r="171" spans="1:8">
+      <c r="A171" s="5"/>
+      <c r="B171" s="5"/>
+      <c r="C171" s="5"/>
+    </row>
+    <row r="172" spans="1:8">
+      <c r="A172" s="5"/>
+      <c r="B172" s="5"/>
+      <c r="C172" s="5"/>
+    </row>
+    <row r="173" spans="1:8">
+      <c r="A173" s="5"/>
+      <c r="B173" s="5"/>
+      <c r="C173" s="5"/>
     </row>
     <row r="174" spans="1:8">
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
-      <c r="H174" s="5"/>
     </row>
     <row r="175" spans="1:8">
       <c r="A175" s="5"/>
@@ -1969,261 +2000,261 @@
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:9">
       <c r="A177" s="5"/>
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:9">
       <c r="A178" s="5"/>
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:9">
       <c r="A179" s="5"/>
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:9">
       <c r="A180" s="5"/>
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:9">
       <c r="A181" s="5"/>
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:9">
       <c r="A182" s="5"/>
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:9">
       <c r="A183" s="5"/>
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
-    </row>
-    <row r="184" spans="1:7">
+      <c r="G183" s="6"/>
+    </row>
+    <row r="184" spans="1:9">
       <c r="A184" s="5"/>
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:9">
       <c r="A185" s="5"/>
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:9">
       <c r="A186" s="5"/>
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
-    </row>
-    <row r="187" spans="1:7">
+      <c r="G186" s="6"/>
+      <c r="H186" s="6"/>
+      <c r="I186" s="6"/>
+    </row>
+    <row r="187" spans="1:9">
       <c r="A187" s="5"/>
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:9">
       <c r="A188" s="5"/>
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:9">
       <c r="A189" s="5"/>
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
     </row>
-    <row r="190" spans="1:7">
-      <c r="A190" s="5"/>
-      <c r="B190" s="5"/>
-      <c r="C190" s="5"/>
-    </row>
-    <row r="191" spans="1:7">
-      <c r="A191" s="5"/>
-      <c r="B191" s="5"/>
-      <c r="C191" s="5"/>
-    </row>
-    <row r="192" spans="1:7">
-      <c r="A192" s="5"/>
-      <c r="B192" s="5"/>
-      <c r="C192" s="5"/>
+    <row r="190" spans="1:9">
+      <c r="A190" s="6"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="6"/>
+    </row>
+    <row r="191" spans="1:9">
+      <c r="A191" s="6"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="6"/>
+      <c r="G191" s="6"/>
+      <c r="H191" s="6"/>
+    </row>
+    <row r="192" spans="1:9">
+      <c r="A192" s="6"/>
+      <c r="B192" s="6"/>
+      <c r="C192" s="6"/>
       <c r="G192" s="6"/>
     </row>
-    <row r="193" spans="1:9">
-      <c r="A193" s="5"/>
-      <c r="B193" s="5"/>
-      <c r="C193" s="5"/>
-    </row>
-    <row r="194" spans="1:9">
-      <c r="A194" s="5"/>
-      <c r="B194" s="5"/>
-      <c r="C194" s="5"/>
-    </row>
-    <row r="195" spans="1:9">
-      <c r="A195" s="5"/>
-      <c r="B195" s="5"/>
-      <c r="C195" s="5"/>
-      <c r="G195" s="6"/>
-      <c r="H195" s="6"/>
-      <c r="I195" s="6"/>
-    </row>
-    <row r="196" spans="1:9">
-      <c r="A196" s="5"/>
-      <c r="B196" s="5"/>
-      <c r="C196" s="5"/>
-    </row>
-    <row r="197" spans="1:9">
-      <c r="A197" s="5"/>
-      <c r="B197" s="5"/>
-      <c r="C197" s="5"/>
-    </row>
-    <row r="198" spans="1:9">
-      <c r="A198" s="5"/>
-      <c r="B198" s="5"/>
-      <c r="C198" s="5"/>
-    </row>
-    <row r="199" spans="1:9">
+    <row r="193" spans="1:10">
+      <c r="A193" s="6"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
+      <c r="G193" s="6"/>
+    </row>
+    <row r="194" spans="1:10">
+      <c r="A194" s="6"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
+      <c r="G194" s="6"/>
+      <c r="H194" s="6"/>
+    </row>
+    <row r="195" spans="1:10">
+      <c r="A195" s="6"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+    </row>
+    <row r="196" spans="1:10">
+      <c r="A196" s="6"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+    </row>
+    <row r="197" spans="1:10">
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="6"/>
+      <c r="G197" s="6"/>
+    </row>
+    <row r="198" spans="1:10">
+      <c r="A198" s="6"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
+      <c r="G198" s="6"/>
+      <c r="H198" s="6"/>
+    </row>
+    <row r="199" spans="1:10">
       <c r="A199" s="6"/>
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:10">
       <c r="A200" s="6"/>
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
-      <c r="G200" s="6"/>
-      <c r="H200" s="6"/>
-    </row>
-    <row r="201" spans="1:9">
+    </row>
+    <row r="201" spans="1:10">
       <c r="A201" s="6"/>
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
       <c r="G201" s="6"/>
-    </row>
-    <row r="202" spans="1:9">
+      <c r="H201" s="6"/>
+      <c r="I201" s="6"/>
+      <c r="J201" s="6"/>
+    </row>
+    <row r="202" spans="1:10">
       <c r="A202" s="6"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
-      <c r="G202" s="6"/>
-    </row>
-    <row r="203" spans="1:9">
+    </row>
+    <row r="203" spans="1:10">
       <c r="A203" s="6"/>
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
-      <c r="G203" s="6"/>
-      <c r="H203" s="6"/>
-    </row>
-    <row r="204" spans="1:9">
+    </row>
+    <row r="204" spans="1:10">
       <c r="A204" s="6"/>
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:10">
       <c r="A205" s="6"/>
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:10">
       <c r="A206" s="6"/>
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
       <c r="G206" s="6"/>
     </row>
-    <row r="207" spans="1:9">
+    <row r="207" spans="1:10">
       <c r="A207" s="6"/>
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
-      <c r="G207" s="6"/>
-      <c r="H207" s="6"/>
-    </row>
-    <row r="208" spans="1:9">
+    </row>
+    <row r="208" spans="1:10">
       <c r="A208" s="6"/>
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:7">
       <c r="A209" s="6"/>
       <c r="B209" s="6"/>
       <c r="C209" s="6"/>
-    </row>
-    <row r="210" spans="1:10">
+      <c r="G209" s="6"/>
+    </row>
+    <row r="210" spans="1:7">
       <c r="A210" s="6"/>
       <c r="B210" s="6"/>
       <c r="C210" s="6"/>
-      <c r="G210" s="6"/>
-      <c r="H210" s="6"/>
-      <c r="I210" s="6"/>
-      <c r="J210" s="6"/>
-    </row>
-    <row r="211" spans="1:10">
+    </row>
+    <row r="211" spans="1:7">
       <c r="A211" s="6"/>
       <c r="B211" s="6"/>
       <c r="C211" s="6"/>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:7">
       <c r="A212" s="6"/>
       <c r="B212" s="6"/>
       <c r="C212" s="6"/>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:7">
       <c r="A213" s="6"/>
       <c r="B213" s="6"/>
       <c r="C213" s="6"/>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:7">
       <c r="A214" s="6"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:7">
       <c r="A215" s="6"/>
       <c r="B215" s="6"/>
       <c r="C215" s="6"/>
-      <c r="G215" s="6"/>
-    </row>
-    <row r="216" spans="1:10">
+    </row>
+    <row r="216" spans="1:7">
       <c r="A216" s="6"/>
       <c r="B216" s="6"/>
       <c r="C216" s="6"/>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:7">
       <c r="A217" s="6"/>
       <c r="B217" s="6"/>
       <c r="C217" s="6"/>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:7">
       <c r="A218" s="6"/>
       <c r="B218" s="6"/>
       <c r="C218" s="6"/>
-      <c r="G218" s="6"/>
-    </row>
-    <row r="219" spans="1:10">
+    </row>
+    <row r="219" spans="1:7">
       <c r="A219" s="6"/>
       <c r="B219" s="6"/>
       <c r="C219" s="6"/>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:7">
       <c r="A220" s="6"/>
       <c r="B220" s="6"/>
       <c r="C220" s="6"/>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:7">
       <c r="A221" s="6"/>
       <c r="B221" s="6"/>
       <c r="C221" s="6"/>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:7">
       <c r="A222" s="6"/>
       <c r="B222" s="6"/>
       <c r="C222" s="6"/>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:7">
       <c r="A223" s="6"/>
       <c r="B223" s="6"/>
       <c r="C223" s="6"/>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:7">
       <c r="A224" s="6"/>
       <c r="B224" s="6"/>
       <c r="C224" s="6"/>
@@ -2237,51 +2268,6 @@
       <c r="A226" s="6"/>
       <c r="B226" s="6"/>
       <c r="C226" s="6"/>
-    </row>
-    <row r="227" spans="1:3">
-      <c r="A227" s="6"/>
-      <c r="B227" s="6"/>
-      <c r="C227" s="6"/>
-    </row>
-    <row r="228" spans="1:3">
-      <c r="A228" s="6"/>
-      <c r="B228" s="6"/>
-      <c r="C228" s="6"/>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="A229" s="6"/>
-      <c r="B229" s="6"/>
-      <c r="C229" s="6"/>
-    </row>
-    <row r="230" spans="1:3">
-      <c r="A230" s="6"/>
-      <c r="B230" s="6"/>
-      <c r="C230" s="6"/>
-    </row>
-    <row r="231" spans="1:3">
-      <c r="A231" s="6"/>
-      <c r="B231" s="6"/>
-      <c r="C231" s="6"/>
-    </row>
-    <row r="232" spans="1:3">
-      <c r="A232" s="6"/>
-      <c r="B232" s="6"/>
-      <c r="C232" s="6"/>
-    </row>
-    <row r="233" spans="1:3">
-      <c r="A233" s="6"/>
-      <c r="B233" s="6"/>
-      <c r="C233" s="6"/>
-    </row>
-    <row r="234" spans="1:3">
-      <c r="A234" s="6"/>
-      <c r="B234" s="6"/>
-      <c r="C234" s="6"/>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235" s="6"/>
-      <c r="B235" s="6"/>
-      <c r="C235" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:C286">

</xml_diff>